<commit_message>
altro fix foto mancanti
</commit_message>
<xml_diff>
--- a/prodotti.xlsx
+++ b/prodotti.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmont\Desktop\Development\PrivateRepo\burger-pizza\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4A02C4-4BF1-4F11-A323-4A021E1A31B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDD349F-EEE4-49F0-B93E-83A3E4699665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-5475" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Antipasti" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="272">
   <si>
     <t>Nome</t>
   </si>
@@ -379,9 +379,6 @@
     <t>american_chips.jpg</t>
   </si>
   <si>
-    <t>chicken_pizza.jpg</t>
-  </si>
-  <si>
     <t>bouquet.jpg</t>
   </si>
   <si>
@@ -694,22 +691,13 @@
     <t>28.00</t>
   </si>
   <si>
-    <t>aperitivo_siciliano.jpg</t>
-  </si>
-  <si>
     <t>AperiBurger</t>
   </si>
   <si>
     <t>30.00</t>
   </si>
   <si>
-    <t>aperiburger.jpg</t>
-  </si>
-  <si>
     <t>AperiPorchetta</t>
-  </si>
-  <si>
-    <t>aperiPorchetta.jpg</t>
   </si>
   <si>
     <r>
@@ -776,33 +764,6 @@
   </si>
   <si>
     <t>Panino greco</t>
-  </si>
-  <si>
-    <t>classico.jpg</t>
-  </si>
-  <si>
-    <t>priolino.jpg</t>
-  </si>
-  <si>
-    <t>appetitoso.jpg</t>
-  </si>
-  <si>
-    <t>goloso.jpg</t>
-  </si>
-  <si>
-    <t>sempliciotto.jpg</t>
-  </si>
-  <si>
-    <t>parigino.jpg</t>
-  </si>
-  <si>
-    <t>fagottino.jpg</t>
-  </si>
-  <si>
-    <t>pizza_cannolo.jpg</t>
-  </si>
-  <si>
-    <t>panino_greco.jpg</t>
   </si>
   <si>
     <t>Pomodoro San Marzano D.O.P., mozzarella fior di latte, prosciutto cotto scelto</t>
@@ -1429,10 +1390,10 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1440,10 +1401,10 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1451,10 +1412,10 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1462,10 +1423,10 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D5" t="s">
         <v>29</v>
@@ -1476,10 +1437,10 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1487,10 +1448,10 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1498,10 +1459,10 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D8" t="s">
         <v>30</v>
@@ -1512,10 +1473,10 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D9" t="s">
         <v>27</v>
@@ -1526,10 +1487,10 @@
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1537,10 +1498,10 @@
         <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1548,10 +1509,10 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1559,10 +1520,10 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1570,10 +1531,10 @@
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1581,10 +1542,10 @@
         <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D15" t="s">
         <v>28</v>
@@ -1595,10 +1556,10 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1633,55 +1594,55 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" t="s">
+        <v>255</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3" t="s">
         <v>196</v>
-      </c>
-      <c r="B3" t="s">
-        <v>268</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="D3" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" t="s">
         <v>194</v>
-      </c>
-      <c r="B4" t="s">
-        <v>199</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D4" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B5" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1716,242 +1677,242 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2" t="s">
         <v>160</v>
       </c>
-      <c r="B2" t="s">
-        <v>161</v>
-      </c>
       <c r="C2" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>166</v>
-      </c>
       <c r="C5" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>176</v>
+      </c>
+      <c r="B17" t="s">
         <v>177</v>
       </c>
-      <c r="B17" t="s">
-        <v>178</v>
-      </c>
       <c r="C17" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B20" t="s">
         <v>179</v>
       </c>
-      <c r="B20" t="s">
-        <v>180</v>
-      </c>
       <c r="C20" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -1963,7 +1924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99B139F4-8144-46BE-9356-F32B8726FE3C}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
@@ -1985,35 +1946,35 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -2026,7 +1987,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2047,44 +2008,35 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C2" t="s">
         <v>214</v>
-      </c>
-      <c r="B2" t="s">
-        <v>252</v>
-      </c>
-      <c r="C2" t="s">
-        <v>215</v>
-      </c>
-      <c r="D2" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B3" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="C3" t="s">
-        <v>218</v>
-      </c>
-      <c r="D3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B4" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="C4" t="s">
-        <v>218</v>
-      </c>
-      <c r="D4" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -2125,10 +2077,10 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2136,10 +2088,10 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2147,10 +2099,10 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2158,10 +2110,10 @@
         <v>11</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2226,12 +2178,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="37" customWidth="1"/>
     <col min="2" max="2" width="61.5703125" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="7"/>
     <col min="4" max="4" width="16.7109375" customWidth="1"/>
@@ -2259,7 +2212,7 @@
         <v>69</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2267,10 +2220,10 @@
         <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2281,7 +2234,7 @@
         <v>70</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -2295,7 +2248,7 @@
         <v>71</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2303,10 +2256,10 @@
         <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D6" t="s">
         <v>106</v>
@@ -2320,7 +2273,7 @@
         <v>72</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2328,10 +2281,10 @@
         <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D8" t="s">
         <v>107</v>
@@ -2345,7 +2298,7 @@
         <v>73</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2356,7 +2309,7 @@
         <v>74</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D10" t="s">
         <v>108</v>
@@ -2370,7 +2323,7 @@
         <v>75</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D11" t="s">
         <v>109</v>
@@ -2384,7 +2337,7 @@
         <v>76</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2395,7 +2348,7 @@
         <v>77</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2406,7 +2359,7 @@
         <v>78</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2417,7 +2370,7 @@
         <v>79</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2428,7 +2381,7 @@
         <v>81</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D16" t="s">
         <v>110</v>
@@ -2442,10 +2395,7 @@
         <v>80</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="D17" t="s">
-        <v>111</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2456,7 +2406,7 @@
         <v>82</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2467,7 +2417,7 @@
         <v>83</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2478,7 +2428,7 @@
         <v>84</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2489,7 +2439,7 @@
         <v>85</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2500,7 +2450,7 @@
         <v>86</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D22" s="4"/>
     </row>
@@ -2542,7 +2492,7 @@
         <v>87</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2553,7 +2503,7 @@
         <v>88</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2564,7 +2514,7 @@
         <v>89</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2575,7 +2525,7 @@
         <v>90</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2586,7 +2536,7 @@
         <v>91</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2597,7 +2547,7 @@
         <v>92</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2640,7 +2590,7 @@
         <v>93</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2651,7 +2601,7 @@
         <v>94</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D3" s="8"/>
     </row>
@@ -2663,7 +2613,7 @@
         <v>95</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2674,7 +2624,7 @@
         <v>96</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2685,7 +2635,7 @@
         <v>97</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2693,10 +2643,10 @@
         <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2707,7 +2657,7 @@
         <v>98</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2718,7 +2668,7 @@
         <v>99</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2729,7 +2679,7 @@
         <v>100</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2740,10 +2690,10 @@
         <v>101</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2754,7 +2704,7 @@
         <v>102</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2765,10 +2715,10 @@
         <v>103</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2779,7 +2729,7 @@
         <v>104</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2790,7 +2740,7 @@
         <v>105</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -2804,7 +2754,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2825,128 +2775,101 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B2" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="D2" t="s">
-        <v>235</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B3" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="D3" t="s">
-        <v>236</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B4" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="D4" t="s">
-        <v>237</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B5" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="D5" t="s">
-        <v>238</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B6" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="D6" t="s">
-        <v>239</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B7" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="D7" t="s">
-        <v>240</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B8" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="D8" t="s">
-        <v>241</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B9" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="D9" t="s">
-        <v>242</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B10" t="s">
         <v>84</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="D10" t="s">
-        <v>243</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2984,160 +2907,160 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B4" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B8" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B9" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B10" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B11" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B12" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B13" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B14" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -3175,102 +3098,102 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
prova foto webP file excel
</commit_message>
<xml_diff>
--- a/prodotti.xlsx
+++ b/prodotti.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmont\Desktop\Development\PrivateRepo\burger-pizza\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A808B46-A4C7-4352-85F4-001238B28EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122D05E2-84F3-4E8B-B486-3F2C35D5FAE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-5475" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>Immagine</t>
   </si>
   <si>
-    <t>margherita.jpg</t>
-  </si>
-  <si>
     <t>Kamut</t>
   </si>
   <si>
@@ -112,18 +109,6 @@
   </si>
   <si>
     <t>Patatine classiche</t>
-  </si>
-  <si>
-    <t>sushi_pizza.jpg</t>
-  </si>
-  <si>
-    <t>arancinette_alla_carne.jpg</t>
-  </si>
-  <si>
-    <t>pata_pig.jpg</t>
-  </si>
-  <si>
-    <t>mangia_e_bevi_di_pizza.jpg</t>
   </si>
   <si>
     <t>Biancaneve</t>
@@ -364,27 +349,6 @@
     <t>Bordo ripieno con crema di pistacchio e philadelphia, mozzarella fior di latte, bresaola, bufala, pomodori secchi, granella di pistacchio</t>
   </si>
   <si>
-    <t>romana.jpg</t>
-  </si>
-  <si>
-    <t>capricciosa.jpg</t>
-  </si>
-  <si>
-    <t>sfiziosa.jpg</t>
-  </si>
-  <si>
-    <t>parmigiana.jpg</t>
-  </si>
-  <si>
-    <t>american_chips.jpg</t>
-  </si>
-  <si>
-    <t>bouquet.jpg</t>
-  </si>
-  <si>
-    <t>duchessa.jpg</t>
-  </si>
-  <si>
     <t>Gigi Burger</t>
   </si>
   <si>
@@ -424,21 +388,6 @@
     <t>Double Cheese Burger</t>
   </si>
   <si>
-    <t>gigi_burger.jpg</t>
-  </si>
-  <si>
-    <t>porchettone.jpg</t>
-  </si>
-  <si>
-    <t>porchi_burger.jpg</t>
-  </si>
-  <si>
-    <t>burger_pig.jpg</t>
-  </si>
-  <si>
-    <t>cheese_burger.jpg</t>
-  </si>
-  <si>
     <t>Pomodoro san marzano D.O.P., mozzarella fior di latte, prosciutto cotto scelto, carciofi, funghi, salame piccante, olive, wurstel, olio evo</t>
   </si>
   <si>
@@ -622,21 +571,12 @@
     <t>1.50</t>
   </si>
   <si>
-    <t>tortino_cuore_caldo.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">Flauto </t>
   </si>
   <si>
-    <t>flauto.jpg</t>
-  </si>
-  <si>
     <t>Zeppola</t>
   </si>
   <si>
-    <t>zeppola.jpg</t>
-  </si>
-  <si>
     <t>Dolce dal cuore morbido e fondente, servito caldo</t>
   </si>
   <si>
@@ -671,18 +611,6 @@
   </si>
   <si>
     <t>20.00</t>
-  </si>
-  <si>
-    <t>pollo_panato_alla_griglia.jpg</t>
-  </si>
-  <si>
-    <t>spiedini_al_pistacchio.jpg</t>
-  </si>
-  <si>
-    <t>spiedini_siciliani.jpg</t>
-  </si>
-  <si>
-    <t>tagliata_di_scottona.jpg</t>
   </si>
   <si>
     <t>Aperitivo siciliano</t>
@@ -944,6 +872,78 @@
   </si>
   <si>
     <t>Buns brioches, hamburger di vitello 150gr, pomodoro, lattuga, mayonese, patatine fritte, 5 nuggets, coca cola</t>
+  </si>
+  <si>
+    <t>margherita.webp</t>
+  </si>
+  <si>
+    <t>romana.webp</t>
+  </si>
+  <si>
+    <t>capricciosa.webp</t>
+  </si>
+  <si>
+    <t>sfiziosa.webp</t>
+  </si>
+  <si>
+    <t>parmigiana.webp</t>
+  </si>
+  <si>
+    <t>american_chips.webp</t>
+  </si>
+  <si>
+    <t>pata_pig.webp</t>
+  </si>
+  <si>
+    <t>mangia_e_bevi_di_pizza.webp</t>
+  </si>
+  <si>
+    <t>sushi_pizza.webp</t>
+  </si>
+  <si>
+    <t>arancinette_alla_carne.webp</t>
+  </si>
+  <si>
+    <t>bouquet.webp</t>
+  </si>
+  <si>
+    <t>duchessa.webp</t>
+  </si>
+  <si>
+    <t>gigi_burger.webp</t>
+  </si>
+  <si>
+    <t>porchettone.webp</t>
+  </si>
+  <si>
+    <t>porchi_burger.webp</t>
+  </si>
+  <si>
+    <t>burger_pig.webp</t>
+  </si>
+  <si>
+    <t>cheese_burger.webp</t>
+  </si>
+  <si>
+    <t>pollo_panato_alla_griglia.webp</t>
+  </si>
+  <si>
+    <t>spiedini_al_pistacchio.webp</t>
+  </si>
+  <si>
+    <t>spiedini_siciliani.webp</t>
+  </si>
+  <si>
+    <t>tagliata_di_scottona.webp</t>
+  </si>
+  <si>
+    <t>tortino_cuore_caldo.webp</t>
+  </si>
+  <si>
+    <t>zeppola.webp</t>
+  </si>
+  <si>
+    <t>flauto.webp</t>
   </si>
 </sst>
 </file>
@@ -1387,179 +1387,179 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>260</v>
+        <v>236</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>261</v>
+        <v>237</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>262</v>
+        <v>238</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>263</v>
+        <v>239</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>264</v>
+        <v>240</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>265</v>
+        <v>241</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>266</v>
+        <v>242</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>257</v>
+        <v>233</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>270</v>
+        <v>246</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>258</v>
+        <v>234</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>259</v>
+        <v>235</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>267</v>
+        <v>243</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>268</v>
+        <v>244</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>269</v>
+        <v>245</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>257</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1594,55 +1594,55 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
       <c r="B2" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="D2" t="s">
-        <v>192</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
       <c r="B3" t="s">
-        <v>255</v>
+        <v>231</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="D3" t="s">
-        <v>196</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
       <c r="B4" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="D4" t="s">
-        <v>194</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
       <c r="B5" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1677,242 +1677,242 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="B2" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="B3" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="B10" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="B11" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="B12" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="B13" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
       <c r="B14" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="B15" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="B17" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
       <c r="B18" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="B19" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
       <c r="B20" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -1946,35 +1946,35 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>218</v>
+        <v>194</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2008,35 +2008,35 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>213</v>
+        <v>189</v>
       </c>
       <c r="B2" t="s">
-        <v>239</v>
+        <v>215</v>
       </c>
       <c r="C2" t="s">
-        <v>214</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>215</v>
+        <v>191</v>
       </c>
       <c r="B3" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
       <c r="C3" t="s">
-        <v>216</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B4" t="s">
         <v>217</v>
       </c>
-      <c r="B4" t="s">
-        <v>241</v>
-      </c>
       <c r="C4" t="s">
-        <v>216</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -2074,46 +2074,46 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2179,7 +2179,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2206,24 +2206,24 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2231,63 +2231,63 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="D6" t="s">
-        <v>106</v>
+        <v>249</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="D8" t="s">
-        <v>107</v>
+        <v>250</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2295,162 +2295,162 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="D10" t="s">
-        <v>108</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="D11" t="s">
-        <v>109</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="D16" t="s">
-        <v>110</v>
+        <v>253</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B17" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B22" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="D22" s="4"/>
     </row>
@@ -2486,46 +2486,46 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2533,21 +2533,21 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -2584,163 +2584,163 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="D11" t="s">
-        <v>111</v>
+        <v>258</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="D13" t="s">
-        <v>112</v>
+        <v>259</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2775,101 +2775,101 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="B2" t="s">
-        <v>231</v>
+        <v>207</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>223</v>
+        <v>199</v>
       </c>
       <c r="B3" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>224</v>
+        <v>200</v>
       </c>
       <c r="B4" t="s">
-        <v>233</v>
+        <v>209</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>225</v>
+        <v>201</v>
       </c>
       <c r="B5" t="s">
-        <v>234</v>
+        <v>210</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>226</v>
+        <v>202</v>
       </c>
       <c r="B6" t="s">
-        <v>235</v>
+        <v>211</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>227</v>
+        <v>203</v>
       </c>
       <c r="B7" t="s">
-        <v>236</v>
+        <v>212</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>228</v>
+        <v>204</v>
       </c>
       <c r="B8" t="s">
-        <v>237</v>
+        <v>213</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
       <c r="B9" t="s">
-        <v>238</v>
+        <v>214</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
       <c r="B10" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2907,160 +2907,160 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>242</v>
+        <v>218</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="D2" t="s">
-        <v>126</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>271</v>
+        <v>247</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>244</v>
+        <v>220</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="D5" t="s">
-        <v>127</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>245</v>
+        <v>221</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="B8" t="s">
-        <v>247</v>
+        <v>223</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="B9" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="B10" t="s">
-        <v>249</v>
+        <v>225</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="D10" t="s">
-        <v>128</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="D11" t="s">
-        <v>129</v>
+        <v>263</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B12" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="B13" t="s">
-        <v>252</v>
+        <v>228</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="D13" t="s">
-        <v>130</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="B14" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -3098,102 +3098,102 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="C3" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="D3" t="s">
-        <v>209</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="C4" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="D4" t="s">
-        <v>210</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="C5" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="D5" t="s">
-        <v>211</v>
+        <v>267</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="C6" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="C7" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="D7" t="s">
-        <v>212</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="C8" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="C9" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>